<commit_message>
update based on ph feedback
</commit_message>
<xml_diff>
--- a/results/2022/sept_report_tables.xlsx
+++ b/results/2022/sept_report_tables.xlsx
@@ -20,12 +20,12 @@
     <sheet name="AIC Model Selection" sheetId="3" r:id="rId6"/>
     <sheet name="Predicted Total Biomass" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="159">
   <si>
     <t>CGOA</t>
   </si>
@@ -521,6 +521,9 @@
   <si>
     <t>4,269 (0.201)</t>
   </si>
+  <si>
+    <t>Percent change from Model 22.1.b</t>
+  </si>
 </sst>
 </file>
 
@@ -528,10 +531,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
-    <numFmt numFmtId="175" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -1054,13 +1057,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1071,29 +1074,29 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="18" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="19" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="18" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1417,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,8 +1595,129 @@
         <v>-6.6135464401485002</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C11" s="20">
+        <v>65630.919166388601</v>
+      </c>
+      <c r="D11" s="20">
+        <v>1968.9275749916501</v>
+      </c>
+      <c r="E11" s="20">
+        <v>1476.69568124374</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C12" s="20">
+        <v>63241.133528352002</v>
+      </c>
+      <c r="D12" s="20">
+        <v>1897.2340058505599</v>
+      </c>
+      <c r="E12" s="20">
+        <v>1422.92550438792</v>
+      </c>
+      <c r="F12" s="25">
+        <v>-3.6412496859565899</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C13" s="20">
+        <v>74108.354914924697</v>
+      </c>
+      <c r="D13" s="20">
+        <v>2223.25064744774</v>
+      </c>
+      <c r="E13" s="20">
+        <v>1667.4379855858001</v>
+      </c>
+      <c r="F13" s="25">
+        <v>12.916832273892</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C14" s="20">
+        <v>71584.055705185194</v>
+      </c>
+      <c r="D14" s="20">
+        <v>2147.5216711555499</v>
+      </c>
+      <c r="E14" s="20">
+        <v>1610.6412533666601</v>
+      </c>
+      <c r="F14" s="25">
+        <v>9.0706280125440895</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C15" s="20">
+        <v>81061.346773603698</v>
+      </c>
+      <c r="D15" s="20">
+        <v>2431.8404032081098</v>
+      </c>
+      <c r="E15" s="20">
+        <v>1823.8803024060801</v>
+      </c>
+      <c r="F15" s="25">
+        <v>23.5109119348086</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3626,7 +3750,7 @@
         <v>5720.74</v>
       </c>
       <c r="E67" s="4">
-        <f t="shared" ref="E67:E91" si="2">(C67-D67)/D67*100</f>
+        <f t="shared" ref="E67:E90" si="2">(C67-D67)/D67*100</f>
         <v>-5.254832258798934E-5</v>
       </c>
       <c r="F67" s="5">
@@ -3636,7 +3760,7 @@
         <v>0.112748878209005</v>
       </c>
       <c r="H67" s="4">
-        <f t="shared" ref="H67:H91" si="3">(F67-G67)/G67*100</f>
+        <f t="shared" ref="H67:H90" si="3">(F67-G67)/G67*100</f>
         <v>-6.4396536046617303E-5</v>
       </c>
     </row>

</xml_diff>